<commit_message>
changed excel sheet added more data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestNG_data.xlsx
+++ b/src/test/resources/testdata/TestNG_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32E864E-C167-4442-A83F-F2D2633D78BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17999386-0CDE-4E9E-840E-5736FD2C9B53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>print("hello")</t>
-  </si>
-  <si>
-    <t>Practice Q1 valid code</t>
   </si>
   <si>
     <t>Element Found
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>Submission Successful</t>
-  </si>
-  <si>
-    <t>Practice Q2 valid code</t>
   </si>
   <si>
     <t>The maximum number of consecutive 1's in input1 is: 
@@ -89,16 +83,10 @@
 1</t>
   </si>
   <si>
-    <t>Practice Q3 valid code</t>
-  </si>
-  <si>
     <t>Even number of digits in given array
 1</t>
   </si>
   <si>
-    <t>Practice Q4 valid code</t>
-  </si>
-  <si>
     <t>[0, 1, 9, 16, 100]
 [4, 9, 9, 49, 121]</t>
   </si>
@@ -163,17 +151,29 @@
     <t>NameError: name 'hello' is not defined on line 1</t>
   </si>
   <si>
-    <t>"def search(lst, value):
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>validRegister</t>
+  </si>
+  <si>
+    <t>PracticeQ1validcode</t>
+  </si>
+  <si>
+    <t>PracticeQ2validcode</t>
+  </si>
+  <si>
+    <t>def search(lst, value):
     if value in lst:
-        return ""Element Found""
+        return "Element Found"
     else:
-        return ""Not Found""
+        return "Not Found"
 # Example usage:
 print(search([12, 23, 45, 67, 6, 90], 12))   # Output: Element Found
-print(search([12, 23, 45, 67, 6, 90], 25))   # Output: Not Found"</t>
-  </si>
-  <si>
-    <t>"def findMaxConsecutiveOnes(nums) :
+print(search([12, 23, 45, 67, 6, 90], 25))   # Output: Not Found</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
   maxCount=0
   currentCount=0
   for n in nums:
@@ -185,35 +185,41 @@
       return maxCount
 input1=[1,1,0,1,1,1]
 input2=[1,0,1,1,0,1]
-print(""The maximum number of consecutive 1's in input1 is: "")
+print("The maximum number of consecutive 1's in input1 is: ")
 print(findMaxConsecutiveOnes(input1))
-print(""The maximum number of consecutive 1's in input2 is: "")
-print(findMaxConsecutiveOnes(input2))"</t>
-  </si>
-  <si>
-    <t>"def findNumbers(nums):
+print("The maximum number of consecutive 1's in input2 is: ")
+print(findMaxConsecutiveOnes(input2))</t>
+  </si>
+  <si>
+    <t>PracticeQ3validcode</t>
+  </si>
+  <si>
+    <t>PracticeQ4validcode</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+  return sorted([x * x for x in nums])
+# Test cases
+print(sortedSquares([-4, -1, 0, 3, 10]))
+print(sortedSquares([-7, -3, 2, 3, 11]))</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
   count = 0
   for num in nums:
     if len(str(num)) % 2 == 0:
       count += 1
       return count
 numsArr1 = [12, 345, 2, 6, 7896]
-print(""Even number of digits in given array"")
-print (findNumbers(numsArr1))"</t>
-  </si>
-  <si>
-    <t>"def sortedSquares(nums):
-  return sorted([x * x for x in nums])
-# Test cases
-print(sortedSquares([-4, -1, 0, 3, 10]))
-print(sortedSquares([-7, -3, 2, 3, 11]))"</t>
+print("Even number of digits in given array")
+print (findNumbers(numsArr1))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +284,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,6 +387,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -671,6 +684,7 @@
     <col min="5" max="5" width="44.08984375" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
     <col min="7" max="7" width="36.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" customWidth="1"/>
     <col min="9" max="9" width="40.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -705,7 +719,7 @@
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -726,7 +740,7 @@
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -743,7 +757,7 @@
     </row>
     <row r="4" spans="1:9" ht="16" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -762,7 +776,7 @@
     </row>
     <row r="5" spans="1:9" ht="16" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -771,7 +785,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -779,7 +793,7 @@
     </row>
     <row r="6" spans="1:9" ht="138" thickBot="1">
       <c r="A6" s="9" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -788,17 +802,17 @@
         <v>45</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="225.5" thickBot="1">
       <c r="A7" s="9" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -807,55 +821,55 @@
         <v>46</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="113" thickBot="1">
       <c r="A8" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="63" thickBot="1">
       <c r="A9" s="9" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="39" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -864,16 +878,16 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="39" thickBot="1">
       <c r="A11" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -881,49 +895,49 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="39" thickBot="1">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="64" thickBot="1">
       <c r="A13" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="39" thickBot="1">
+    <row r="14" spans="1:9" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -932,16 +946,16 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="14" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="39" thickBot="1">
+    <row r="15" spans="1:9" ht="16" thickBot="1">
       <c r="A15" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -949,13 +963,13 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="14" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="39" thickBot="1">
+    <row r="16" spans="1:9" ht="16" thickBot="1">
       <c r="A16" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
@@ -966,16 +980,16 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="14" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="39" thickBot="1">
+    <row r="17" spans="1:9" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>10</v>
@@ -985,16 +999,16 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="14" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" ht="39" thickBot="1">
+    <row r="18" spans="1:9" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -1004,10 +1018,24 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16.5">
+      <c r="A19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted a dependecny in pom.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestNG_data.xlsx
+++ b/src/test/resources/testdata/TestNG_data.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17999386-0CDE-4E9E-840E-5736FD2C9B53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B099C6-D5B1-4F06-BB0F-DC66BB48BFB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="practiceQ" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -94,9 +95,6 @@
     <t>Login1</t>
   </si>
   <si>
-    <t>Please fill out this field</t>
-  </si>
-  <si>
     <t>Login2</t>
   </si>
   <si>
@@ -128,9 +126,6 @@
   </si>
   <si>
     <t>Register5</t>
-  </si>
-  <si>
-    <t>missmathch password</t>
   </si>
   <si>
     <t>abcdef</t>
@@ -204,22 +199,23 @@
 print(sortedSquares([-7, -3, 2, 3, 11]))</t>
   </si>
   <si>
-    <t>def findNumbers(nums):
-  count = 0
-  for num in nums:
-    if len(str(num)) % 2 == 0:
-      count += 1
-      return count
-numsArr1 = [12, 345, 2, 6, 7896]
-print("Even number of digits in given array")
-print (findNumbers(numsArr1))</t>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>EmptyCode</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>user is already registered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,16 +257,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Play"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arimo"/>
     </font>
     <font>
       <sz val="10"/>
@@ -341,9 +327,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,7 +340,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -372,22 +358,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -669,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -688,7 +668,7 @@
     <col min="9" max="9" width="40.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +699,7 @@
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -740,7 +720,7 @@
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -757,7 +737,7 @@
     </row>
     <row r="4" spans="1:9" ht="16" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -776,7 +756,7 @@
     </row>
     <row r="5" spans="1:9" ht="16" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -785,256 +765,208 @@
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="138" thickBot="1">
-      <c r="A6" s="9" t="s">
-        <v>43</v>
+    <row r="6" spans="1:9" ht="16" thickBot="1">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="225.5" thickBot="1">
+    <row r="7" spans="1:9" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="113" thickBot="1">
+    <row r="8" spans="1:9" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" ht="63" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="39" thickBot="1">
+    <row r="10" spans="1:9" ht="26.5" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="39" thickBot="1">
+    <row r="11" spans="1:9" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="5" t="s">
-        <v>22</v>
+      <c r="H11" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" ht="39" thickBot="1">
+    <row r="12" spans="1:9" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="5" t="s">
-        <v>22</v>
+      <c r="H12" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" ht="64" thickBot="1">
+    <row r="13" spans="1:9" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="5" t="s">
-        <v>28</v>
+      <c r="H13" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="14" t="s">
-        <v>41</v>
+      <c r="H14" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="16" thickBot="1">
+    <row r="15" spans="1:9" ht="50" thickBot="1">
       <c r="A15" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="14" t="s">
-        <v>41</v>
+      <c r="H15" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="16" thickBot="1">
-      <c r="A16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5" t="s">
+    <row r="16" spans="1:9" ht="17" thickBot="1">
+      <c r="A16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="14" t="s">
-        <v>41</v>
+      <c r="H16" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="16" thickBot="1">
-      <c r="A17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="14" t="s">
-        <v>41</v>
-      </c>
+    <row r="17" spans="9:9" ht="16" thickBot="1">
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" ht="16" thickBot="1">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="9:9" ht="16" thickBot="1">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="9:9" ht="16" thickBot="1">
+      <c r="I19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16.5">
-      <c r="A19" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="15" t="s">
+    </row>
+    <row r="20" spans="9:9" ht="16.5">
+      <c r="I20" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1046,4 +978,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13D2D43-A4DE-453E-B214-1EDE512C27EB}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="45.36328125" customWidth="1"/>
+    <col min="2" max="2" width="42.6328125" customWidth="1"/>
+    <col min="3" max="3" width="46.6328125" customWidth="1"/>
+    <col min="4" max="4" width="38.08984375" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="275.5">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="58">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated the excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestNG_data.xlsx
+++ b/src/test/resources/testdata/TestNG_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B099C6-D5B1-4F06-BB0F-DC66BB48BFB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CEA7A1-DE9F-4EE6-AC39-E036B948853E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -76,16 +76,6 @@
   </si>
   <si>
     <t>Submission Successful</t>
-  </si>
-  <si>
-    <t>The maximum number of consecutive 1's in input1 is: 
-2
-The maximum number of consecutive 1's in input2 is: 
-1</t>
-  </si>
-  <si>
-    <t>Even number of digits in given array
-1</t>
   </si>
   <si>
     <t>[0, 1, 9, 16, 100]
@@ -168,24 +158,6 @@
 print(search([12, 23, 45, 67, 6, 90], 25))   # Output: Not Found</t>
   </si>
   <si>
-    <t>def findMaxConsecutiveOnes(nums) :
-  maxCount=0
-  currentCount=0
-  for n in nums:
-    if(n==1):
-      currentCount+=1
-      maxCount=max(maxCount,currentCount)
-    else:
-      currentCount=0
-      return maxCount
-input1=[1,1,0,1,1,1]
-input2=[1,0,1,1,0,1]
-print("The maximum number of consecutive 1's in input1 is: ")
-print(findMaxConsecutiveOnes(input1))
-print("The maximum number of consecutive 1's in input2 is: ")
-print(findMaxConsecutiveOnes(input2))</t>
-  </si>
-  <si>
     <t>PracticeQ3validcode</t>
   </si>
   <si>
@@ -209,6 +181,43 @@
   </si>
   <si>
     <t>user is already registered</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0  # reset when 0 is found
+    return max_count
+# Example usage:
+print(findMaxConsecutiveOnes([1,1,0,1,1,1]))  # Output: 3
+print(findMaxConsecutiveOnes([1,0,1,1,0,1]))  # Output: 2</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+# Example usage:
+print(findNumbers([12, 345, 2, 6, 7896]))   # Output: 2
+print(findNumbers([555, 901, 482, 1771]))  # Output: 1</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>3
+2</t>
+  </si>
+  <si>
+    <t>2
+1</t>
   </si>
 </sst>
 </file>
@@ -329,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,6 +376,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -699,7 +714,7 @@
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -720,7 +735,7 @@
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -737,7 +752,7 @@
     </row>
     <row r="4" spans="1:9" ht="16" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -756,7 +771,7 @@
     </row>
     <row r="5" spans="1:9" ht="16" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -765,7 +780,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -773,7 +788,7 @@
     </row>
     <row r="6" spans="1:9" ht="16" thickBot="1">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -786,7 +801,7 @@
     </row>
     <row r="7" spans="1:9" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -795,16 +810,16 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -812,49 +827,49 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="26.5" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -863,16 +878,16 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -880,13 +895,13 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
@@ -897,16 +912,16 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
@@ -916,16 +931,16 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="50" thickBot="1">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
@@ -935,13 +950,13 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1">
       <c r="A16" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>9</v>
@@ -950,7 +965,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I16" s="6"/>
     </row>
@@ -962,7 +977,7 @@
     </row>
     <row r="19" spans="9:9" ht="16" thickBot="1">
       <c r="I19" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="9:9" ht="16.5">
@@ -982,103 +997,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13D2D43-A4DE-453E-B214-1EDE512C27EB}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="45.36328125" customWidth="1"/>
-    <col min="2" max="2" width="42.6328125" customWidth="1"/>
+    <col min="2" max="2" width="52.453125" customWidth="1"/>
     <col min="3" max="3" width="46.6328125" customWidth="1"/>
     <col min="4" max="4" width="38.08984375" customWidth="1"/>
     <col min="5" max="5" width="33.81640625" customWidth="1"/>
     <col min="6" max="6" width="14.90625" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="275.5">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="275.5">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="58">
+    <row r="4" spans="1:7" ht="29">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated changes in modules
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestNG_data.xlsx
+++ b/src/test/resources/testdata/TestNG_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CEA7A1-DE9F-4EE6-AC39-E036B948853E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D856581-4A51-41B1-9A0C-A9C0103BA8F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -218,6 +218,12 @@
   <si>
     <t>2
 1</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13D2D43-A4DE-453E-B214-1EDE512C27EB}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1012,9 +1018,10 @@
     <col min="5" max="5" width="33.81640625" customWidth="1"/>
     <col min="6" max="6" width="14.90625" customWidth="1"/>
     <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="36.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1036,8 +1043,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="275.5">
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="275.5">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1057,7 +1067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29">
+    <row r="4" spans="1:8" ht="58">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1087,8 +1097,11 @@
       <c r="G4" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H4" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="D6" s="15"/>
     </row>
   </sheetData>

</xml_diff>